<commit_message>
EPIC emv configuration bundles added
</commit_message>
<xml_diff>
--- a/Documentation/DecToHex_Conversion_Table.xlsx
+++ b/Documentation/DecToHex_Conversion_Table.xlsx
@@ -339,7 +339,7 @@
   <dimension ref="B1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C1" sqref="C1:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -349,74 +349,74 @@
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B1">
-        <v>67538</v>
+        <v>66661</v>
       </c>
       <c r="C1" t="str">
         <f>DEC2HEX($B1,8)</f>
-        <v>000107D2</v>
+        <v>00010465</v>
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>67311</v>
+        <v>66782</v>
       </c>
       <c r="C2" t="str">
         <f>DEC2HEX($B2,8)</f>
-        <v>000106EF</v>
+        <v>000104DE</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>67542</v>
+        <v>66663</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C8" si="0">DEC2HEX($B3,8)</f>
-        <v>000107D6</v>
+        <v>00010467</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>67552</v>
+        <v>66666</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
-        <v>000107E0</v>
+        <v>0001046A</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>67403</v>
+        <v>66511</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
-        <v>0001074B</v>
+        <v>000103CF</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>67415</v>
+        <v>66444</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
-        <v>00010757</v>
+        <v>0001038C</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>67002</v>
+        <v>66757</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
-        <v>000105BA</v>
+        <v>000104C5</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>67504</v>
+        <v>66469</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
-        <v>000107B0</v>
+        <v>000103A5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>